<commit_message>
fixes for the formula if the player lost the match
</commit_message>
<xml_diff>
--- a/src/main/java/tournamentFiles/Tournament.xlsx
+++ b/src/main/java/tournamentFiles/Tournament.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>Participantes</t>
   </si>
@@ -75,9 +75,6 @@
     <t>Franco Banfi</t>
   </si>
   <si>
-    <t>Jugador</t>
-  </si>
-  <si>
     <t>Gaston Dupertuis</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
   </si>
   <si>
     <t>hasta 24</t>
-  </si>
-  <si>
-    <t>Contrincate</t>
   </si>
   <si>
     <t>Javier Tenca</t>
@@ -937,7 +931,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4">
         <v>604</v>
@@ -967,7 +961,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4">
         <v>174</v>
@@ -997,7 +991,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4">
         <v>100</v>
@@ -1027,7 +1021,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>100</v>
@@ -1087,7 +1081,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4">
         <v>943</v>
@@ -1117,7 +1111,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="4">
         <v>100</v>
@@ -1147,7 +1141,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="4">
         <v>100</v>
@@ -1177,7 +1171,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="4">
         <v>150</v>
@@ -1207,7 +1201,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4">
         <v>100</v>
@@ -1237,7 +1231,7 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B20" s="4">
         <v>128</v>
@@ -1267,7 +1261,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B21" s="4">
         <v>70</v>
@@ -1297,7 +1291,7 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="4">
         <v>70</v>
@@ -1327,7 +1321,7 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4">
         <v>70</v>
@@ -1357,7 +1351,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="4">
         <v>50</v>
@@ -1387,7 +1381,7 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" s="4">
         <v>70</v>
@@ -1417,7 +1411,7 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B26" s="4">
         <v>62</v>
@@ -1447,7 +1441,7 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B27" s="4">
         <v>70</v>
@@ -1477,7 +1471,7 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B28" s="4">
         <v>70</v>
@@ -1507,7 +1501,7 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" s="4">
         <v>50</v>
@@ -1537,7 +1531,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" s="4">
         <v>50</v>
@@ -1567,7 +1561,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="4">
         <v>50</v>
@@ -1597,7 +1591,7 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B32" s="4">
         <v>50</v>
@@ -1627,7 +1621,7 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B33" s="4">
         <v>50</v>
@@ -1657,7 +1651,7 @@
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4">
         <v>50</v>
@@ -1687,7 +1681,7 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B35" s="4">
         <v>50</v>
@@ -1717,7 +1711,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="4">
         <v>50</v>
@@ -1747,7 +1741,7 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B37" s="4">
         <v>50</v>
@@ -1777,7 +1771,7 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B38" s="4">
         <v>50</v>
@@ -1807,7 +1801,7 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B39" s="4">
         <v>50</v>
@@ -1837,7 +1831,7 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B40" s="4">
         <v>50</v>
@@ -1867,7 +1861,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B41" s="4">
         <v>50</v>
@@ -1897,7 +1891,7 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B42" s="4">
         <v>50</v>
@@ -1927,7 +1921,7 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B43" s="4">
         <v>50</v>
@@ -1957,7 +1951,7 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1">
       <c r="A44" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B44" s="4">
         <v>50</v>
@@ -1987,7 +1981,7 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1">
       <c r="A45" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B45" s="4">
         <v>50</v>
@@ -2017,7 +2011,7 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1">
       <c r="A46" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B46" s="4">
         <v>50</v>
@@ -2047,7 +2041,7 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1">
       <c r="A47" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="4">
         <v>50</v>
@@ -2077,7 +2071,7 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1">
       <c r="A48" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B48" s="4">
         <v>50</v>
@@ -2289,7 +2283,7 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1">
       <c r="A56" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -26843,7 +26837,7 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -26920,7 +26914,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>5</v>
@@ -26940,7 +26934,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>5</v>
@@ -26960,7 +26954,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>5</v>
@@ -27040,10 +27034,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>19</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D9" s="4">
         <v>270</v>
@@ -27060,10 +27054,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D10" s="4">
         <v>270</v>
@@ -27080,10 +27074,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>19</v>
+        <v>32</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D11" s="4">
         <v>270</v>
@@ -27100,10 +27094,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="D12" s="4">
         <v>270</v>
@@ -27123,7 +27117,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="D13" s="4">
         <v>270</v>
@@ -27140,10 +27134,10 @@
         <v>7</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D14" s="4">
         <v>493</v>
@@ -27160,10 +27154,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>19</v>
+        <v>36</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D15" s="4">
         <v>493</v>
@@ -27180,10 +27174,10 @@
         <v>7</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="4">
         <v>493</v>
@@ -27202,8 +27196,8 @@
       <c r="B17" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>19</v>
+      <c r="C17" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D17" s="4">
         <v>493</v>
@@ -27223,7 +27217,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D18" s="4">
         <v>493</v>
@@ -27240,10 +27234,10 @@
         <v>8</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D19" s="4">
         <v>386</v>
@@ -27260,10 +27254,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>19</v>
+        <v>50</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D20" s="4">
         <v>386</v>
@@ -27280,10 +27274,10 @@
         <v>8</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>19</v>
+        <v>51</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="D21" s="4">
         <v>386</v>
@@ -27303,7 +27297,7 @@
         <v>7</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="D22" s="4">
         <v>386</v>
@@ -27338,18 +27332,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" s="11">
         <v>18</v>
@@ -27360,7 +27354,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="11">
         <v>16</v>
@@ -27371,7 +27365,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="11">
         <v>14</v>
@@ -27382,7 +27376,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B7" s="11">
         <v>12</v>
@@ -27393,7 +27387,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="11">
         <v>10</v>
@@ -27404,7 +27398,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B9" s="11">
         <v>8</v>
@@ -27415,7 +27409,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="11">
         <v>6</v>
@@ -27426,7 +27420,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="11">
         <v>4</v>
@@ -27437,7 +27431,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="11">
         <v>2</v>
@@ -27448,7 +27442,7 @@
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B13" s="11">
         <v>0</v>
@@ -27459,28 +27453,28 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>27</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="11">
         <v>18</v>
@@ -27491,7 +27485,7 @@
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="11">
         <v>22</v>
@@ -27502,7 +27496,7 @@
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="11">
         <v>26</v>
@@ -27513,7 +27507,7 @@
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" s="11">
         <v>30</v>
@@ -27524,7 +27518,7 @@
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B24" s="11">
         <v>36</v>
@@ -27535,7 +27529,7 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="11">
         <v>42</v>
@@ -27546,7 +27540,7 @@
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" s="11">
         <v>48</v>
@@ -27557,7 +27551,7 @@
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27" s="11">
         <v>56</v>
@@ -27568,7 +27562,7 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B28" s="11">
         <v>64</v>
@@ -27579,7 +27573,7 @@
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
       <c r="A29" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B29" s="11">
         <v>80</v>

</xml_diff>

<commit_message>
- Write data methods to output the result on the Tournament .xlsx file Realease V1.0 done!
</commit_message>
<xml_diff>
--- a/src/main/java/tournamentFiles/Tournament.xlsx
+++ b/src/main/java/tournamentFiles/Tournament.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -637,16 +637,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -689,7 +689,7 @@
         <v>378</v>
       </c>
       <c r="C2" s="4">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="D2" s="5"/>
       <c r="G2" s="3"/>
@@ -721,7 +721,7 @@
         <v>270</v>
       </c>
       <c r="C3" s="4">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D3" s="5"/>
       <c r="G3" s="3"/>
@@ -753,7 +753,7 @@
         <v>493</v>
       </c>
       <c r="C4" s="4">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="D4" s="5"/>
       <c r="G4" s="3"/>
@@ -778,15 +778,13 @@
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>386</v>
       </c>
-      <c r="C5" s="4">
-        <v>503</v>
-      </c>
+      <c r="C5" s="4"/>
       <c r="D5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -26836,16 +26834,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -26905,7 +26903,6 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <f>8</f>
         <v>8</v>
       </c>
     </row>
@@ -26986,7 +26983,7 @@
         <v>270</v>
       </c>
       <c r="F6" s="8">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
@@ -27045,9 +27042,7 @@
       <c r="E9" s="4">
         <v>70</v>
       </c>
-      <c r="F9" s="8">
-        <v>8</v>
-      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
@@ -27065,9 +27060,7 @@
       <c r="E10" s="8">
         <v>50</v>
       </c>
-      <c r="F10" s="8">
-        <v>8</v>
-      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
@@ -27085,9 +27078,7 @@
       <c r="E11" s="8">
         <v>70</v>
       </c>
-      <c r="F11" s="8">
-        <v>8</v>
-      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
@@ -27105,9 +27096,7 @@
       <c r="E12" s="8">
         <v>70</v>
       </c>
-      <c r="F12" s="8">
-        <v>8</v>
-      </c>
+      <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
@@ -27125,9 +27114,7 @@
       <c r="E13" s="4">
         <v>378</v>
       </c>
-      <c r="F13" s="8">
-        <v>-8</v>
-      </c>
+      <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
@@ -27145,9 +27132,7 @@
       <c r="E14" s="4">
         <v>174</v>
       </c>
-      <c r="F14" s="8">
-        <v>4</v>
-      </c>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
@@ -27165,9 +27150,7 @@
       <c r="E15" s="8">
         <v>50</v>
       </c>
-      <c r="F15" s="8">
-        <v>4</v>
-      </c>
+      <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
@@ -27185,9 +27168,7 @@
       <c r="E16" s="8">
         <v>50</v>
       </c>
-      <c r="F16" s="8">
-        <v>4</v>
-      </c>
+      <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
@@ -27205,9 +27186,7 @@
       <c r="E17" s="4">
         <v>386</v>
       </c>
-      <c r="F17" s="8">
-        <v>10</v>
-      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
@@ -27225,9 +27204,7 @@
       <c r="E18" s="4">
         <v>544</v>
       </c>
-      <c r="F18" s="8">
-        <v>-14</v>
-      </c>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
@@ -27245,9 +27222,7 @@
       <c r="E19" s="8">
         <v>100</v>
       </c>
-      <c r="F19" s="8">
-        <v>8</v>
-      </c>
+      <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
@@ -27265,9 +27240,7 @@
       <c r="E20" s="8">
         <v>50</v>
       </c>
-      <c r="F20" s="8">
-        <v>6</v>
-      </c>
+      <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -27285,9 +27258,7 @@
       <c r="E21" s="8">
         <v>50</v>
       </c>
-      <c r="F21" s="8">
-        <v>6</v>
-      </c>
+      <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -27305,9 +27276,7 @@
       <c r="E22" s="4">
         <v>493</v>
       </c>
-      <c r="F22" s="8">
-        <v>-10</v>
-      </c>
+      <c r="F22" s="8"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="3"/>
@@ -27330,7 +27299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" s="10" t="s">
         <v>22</v>
       </c>
@@ -27451,7 +27420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" s="12" t="s">
         <v>48</v>
       </c>
@@ -27461,7 +27430,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" ht="15">
       <c r="A19" s="10" t="s">
         <v>22</v>
       </c>

</xml_diff>